<commit_message>
support blank row and colum start
</commit_message>
<xml_diff>
--- a/DiffExcel/Test/DiffExcelBDD.xlsx
+++ b/DiffExcel/Test/DiffExcelBDD.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Code\ExcelBDD\DiffExcel\Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BB535A7-D7BF-40BB-80FA-C26B86538A63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A4C1C3D-9DF4-4BFF-99CB-136316BAF0C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{513EC524-C410-4B00-B12F-D02046789CA3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{513EC524-C410-4B00-B12F-D02046789CA3}"/>
   </bookViews>
   <sheets>
     <sheet name="DiffExcel" sheetId="1" r:id="rId1"/>
+    <sheet name="DiffWorksheet" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="52">
   <si>
     <t>Step</t>
   </si>
@@ -99,6 +100,96 @@
   </si>
   <si>
     <t>OldFile.xlsx</t>
+  </si>
+  <si>
+    <t>Set inputs</t>
+  </si>
+  <si>
+    <t>WorksheetName</t>
+  </si>
+  <si>
+    <t>Sheet1</t>
+  </si>
+  <si>
+    <t>ResultType</t>
+  </si>
+  <si>
+    <t>Object[]</t>
+  </si>
+  <si>
+    <t>DiffCount</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>B1   OldB1 NewB1</t>
+  </si>
+  <si>
+    <t>ResultNum1</t>
+  </si>
+  <si>
+    <t>ResultText1</t>
+  </si>
+  <si>
+    <t>Check comparision</t>
+  </si>
+  <si>
+    <t>ResultNum2</t>
+  </si>
+  <si>
+    <t>ResultText2</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>B3   NewB3 B3</t>
+  </si>
+  <si>
+    <t>ResultNum3</t>
+  </si>
+  <si>
+    <t>ResultText3</t>
+  </si>
+  <si>
+    <t>C10  OldC10</t>
+  </si>
+  <si>
+    <t>Scenario2</t>
+  </si>
+  <si>
+    <t>Sheet2</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>B11  OldB11</t>
+  </si>
+  <si>
+    <t>C1   OldC1</t>
+  </si>
+  <si>
+    <t>C11  OldC11</t>
+  </si>
+  <si>
+    <t>Scenario3</t>
+  </si>
+  <si>
+    <t>Sheet3</t>
+  </si>
+  <si>
+    <t>G13      NewG13</t>
+  </si>
+  <si>
+    <t>F14      NewF14</t>
+  </si>
+  <si>
+    <t>G14      NewG14</t>
   </si>
 </sst>
 </file>
@@ -156,7 +247,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -179,11 +270,42 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -201,10 +323,22 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -522,8 +656,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23C6FFDF-A533-45DE-AE30-7B256E237E30}">
   <dimension ref="A4:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D6" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -553,7 +687,7 @@
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="9" t="s">
         <v>18</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -570,7 +704,7 @@
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="7"/>
+      <c r="A6" s="9"/>
       <c r="B6" s="4" t="s">
         <v>17</v>
       </c>
@@ -585,7 +719,7 @@
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="10" t="s">
         <v>19</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -602,8 +736,8 @@
       </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="8"/>
-      <c r="B8" s="9" t="s">
+      <c r="A8" s="10"/>
+      <c r="B8" s="8" t="s">
         <v>10</v>
       </c>
       <c r="C8" s="4" t="s">
@@ -617,8 +751,8 @@
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="8"/>
-      <c r="B9" s="9"/>
+      <c r="A9" s="10"/>
+      <c r="B9" s="8"/>
       <c r="C9" s="4" t="s">
         <v>13</v>
       </c>
@@ -630,8 +764,8 @@
       </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="8"/>
-      <c r="B10" s="9"/>
+      <c r="A10" s="10"/>
+      <c r="B10" s="8"/>
       <c r="C10" s="4" t="s">
         <v>13</v>
       </c>
@@ -651,4 +785,183 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5649DE3-DFCC-48C8-A239-58F58924BEB5}">
+  <dimension ref="A4:E13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="34.5703125" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="19.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="1:5">
+      <c r="A4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="12"/>
+      <c r="B7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="5">
+        <v>24</v>
+      </c>
+      <c r="D7" s="5">
+        <v>3</v>
+      </c>
+      <c r="E7" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="12"/>
+      <c r="B8" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="12"/>
+      <c r="B9" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="12"/>
+      <c r="B10" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="12"/>
+      <c r="B11" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="12"/>
+      <c r="B12" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="13"/>
+      <c r="B13" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A6:A13"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update DiffExcel to V1.2
</commit_message>
<xml_diff>
--- a/DiffExcel/Test/DiffExcelBDD.xlsx
+++ b/DiffExcel/Test/DiffExcelBDD.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Code\ExcelBDD\DiffExcel\Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FEC39FB-2559-41E3-9533-AC281A407963}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D63BEB0-85AC-44D9-B12A-0198D58AD991}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{513EC524-C410-4B00-B12F-D02046789CA3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{513EC524-C410-4B00-B12F-D02046789CA3}"/>
   </bookViews>
   <sheets>
     <sheet name="DiffExcel" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="48">
   <si>
     <t>Step</t>
   </si>
@@ -163,6 +163,21 @@
   </si>
   <si>
     <t>G14      NewG14</t>
+  </si>
+  <si>
+    <t>Scenario4</t>
+  </si>
+  <si>
+    <t>Sheet4</t>
+  </si>
+  <si>
+    <t>A1   OldA1</t>
+  </si>
+  <si>
+    <t>B1   OldB1</t>
+  </si>
+  <si>
+    <t>A2   OldA2</t>
   </si>
 </sst>
 </file>
@@ -629,7 +644,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23C6FFDF-A533-45DE-AE30-7B256E237E30}">
   <dimension ref="A4:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
@@ -732,20 +747,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5649DE3-DFCC-48C8-A239-58F58924BEB5}">
-  <dimension ref="A4:E13"/>
+  <dimension ref="A4:F13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="34.5703125" customWidth="1"/>
     <col min="2" max="2" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="19.42578125" customWidth="1"/>
+    <col min="3" max="6" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -761,8 +776,11 @@
       <c r="E4" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="F4" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" s="7" t="s">
         <v>13</v>
       </c>
@@ -778,8 +796,11 @@
       <c r="E5" s="5" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="F5" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" s="11" t="s">
         <v>23</v>
       </c>
@@ -795,8 +816,11 @@
       <c r="E6" s="5" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="F6" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" s="12"/>
       <c r="B7" s="3" t="s">
         <v>18</v>
@@ -810,8 +834,11 @@
       <c r="E7" s="5">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="F7" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" s="12"/>
       <c r="B8" s="3" t="s">
         <v>21</v>
@@ -825,8 +852,11 @@
       <c r="E8" s="6" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="F8" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" s="12"/>
       <c r="B9" s="3" t="s">
         <v>22</v>
@@ -840,8 +870,11 @@
       <c r="E9" s="5" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="10" spans="1:5">
+      <c r="F9" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" s="12"/>
       <c r="B10" s="3" t="s">
         <v>24</v>
@@ -855,8 +888,11 @@
       <c r="E10" s="6" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="11" spans="1:5">
+      <c r="F10" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" s="12"/>
       <c r="B11" s="3" t="s">
         <v>25</v>
@@ -870,8 +906,11 @@
       <c r="E11" s="6" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="12" spans="1:5">
+      <c r="F11" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" s="12"/>
       <c r="B12" s="3" t="s">
         <v>29</v>
@@ -885,8 +924,11 @@
       <c r="E12" s="6" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="13" spans="1:5">
+      <c r="F12" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" s="13"/>
       <c r="B13" s="3" t="s">
         <v>30</v>
@@ -899,6 +941,9 @@
       </c>
       <c r="E13" s="6" t="s">
         <v>42</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
diffexcel and support junit4
</commit_message>
<xml_diff>
--- a/DiffExcel/Test/DiffExcelBDD.xlsx
+++ b/DiffExcel/Test/DiffExcelBDD.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Code\ExcelBDD\DiffExcel\Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D63BEB0-85AC-44D9-B12A-0198D58AD991}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1796D37-8960-4883-B801-DC32483F517C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{513EC524-C410-4B00-B12F-D02046789CA3}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="40">
   <si>
     <t>Step</t>
   </si>
@@ -84,63 +84,21 @@
     <t>Sheet1</t>
   </si>
   <si>
-    <t>ResultType</t>
-  </si>
-  <si>
-    <t>Object[]</t>
-  </si>
-  <si>
     <t>DiffCount</t>
   </si>
   <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>B1   OldB1 NewB1</t>
-  </si>
-  <si>
-    <t>ResultNum1</t>
-  </si>
-  <si>
     <t>ResultText1</t>
   </si>
   <si>
-    <t>Check comparision</t>
-  </si>
-  <si>
-    <t>ResultNum2</t>
-  </si>
-  <si>
     <t>ResultText2</t>
   </si>
   <si>
-    <t>23</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>B3   NewB3 B3</t>
-  </si>
-  <si>
-    <t>ResultNum3</t>
-  </si>
-  <si>
-    <t>ResultText3</t>
-  </si>
-  <si>
-    <t>C10  OldC10</t>
-  </si>
-  <si>
     <t>Scenario2</t>
   </si>
   <si>
     <t>Sheet2</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
     <t>B11  OldB11</t>
   </si>
   <si>
@@ -178,6 +136,24 @@
   </si>
   <si>
     <t>A2   OldA2</t>
+  </si>
+  <si>
+    <t>ResultText0</t>
+  </si>
+  <si>
+    <t>A1   A1  NewA1</t>
+  </si>
+  <si>
+    <t>B6   B6  NewB6</t>
+  </si>
+  <si>
+    <t>C11  C11 NewC11</t>
+  </si>
+  <si>
+    <t>Parameter Name</t>
+  </si>
+  <si>
+    <t>Check comparison results</t>
   </si>
 </sst>
 </file>
@@ -235,7 +211,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -263,17 +239,6 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -293,7 +258,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -320,13 +285,10 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -747,17 +709,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5649DE3-DFCC-48C8-A239-58F58924BEB5}">
-  <dimension ref="A4:F13"/>
+  <dimension ref="A4:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="34.5703125" customWidth="1"/>
-    <col min="2" max="2" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="6" width="19.42578125" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="1:6">
@@ -765,19 +730,19 @@
         <v>0</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>43</v>
+      <c r="D4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -791,165 +756,94 @@
         <v>15</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="11" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="5">
+        <v>3</v>
+      </c>
+      <c r="D6" s="5">
+        <v>3</v>
+      </c>
+      <c r="E6" s="5">
+        <v>3</v>
+      </c>
+      <c r="F6" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="11"/>
+      <c r="B7" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="11"/>
+      <c r="B8" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="12"/>
-      <c r="B7" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="5">
-        <v>24</v>
-      </c>
-      <c r="D7" s="5">
-        <v>3</v>
-      </c>
-      <c r="E7" s="5">
-        <v>3</v>
-      </c>
-      <c r="F7" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="12"/>
-      <c r="B8" s="3" t="s">
-        <v>21</v>
-      </c>
       <c r="C8" s="6" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="12"/>
       <c r="B9" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="12"/>
-      <c r="B10" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="12"/>
-      <c r="B11" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D11" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="12"/>
-      <c r="B12" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="13"/>
-      <c r="B13" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>47</v>
+      <c r="F9" s="6" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A6:A13"/>
+    <mergeCell ref="A6:A9"/>
   </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>